<commit_message>
Change target field name
</commit_message>
<xml_diff>
--- a/sample_workbooks/sample_workbook.xlsx
+++ b/sample_workbooks/sample_workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juttum/sample workbook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juttum/CAT_Digital/Repos/FOR_POC/P-DH-Sample-Mapping-Documents/sample_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F8E1BD7-C2CD-CF43-894A-E0F100DE6489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE71499F-1FC9-8341-BDB7-5024CDB9C1AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{AF8A8CB7-8D05-7948-8B0B-56E02A934EB1}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>SerialNumber</t>
   </si>
   <si>
-    <t>sno</t>
-  </si>
-  <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>seno</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,16 +442,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
       <c r="F2">
         <v>10</v>

</xml_diff>